<commit_message>
adding reflection code for datadriven test
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -62,16 +56,44 @@
   </si>
   <si>
     <t>p3</t>
+  </si>
+  <si>
+    <t>TC3_twitLoginChrome</t>
+  </si>
+  <si>
+    <t>DatadrivenTest</t>
+  </si>
+  <si>
+    <t>AppURL</t>
+  </si>
+  <si>
+    <t>https://twitter.com/login?lang=en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,13 +116,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,86 +436,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to reflection code
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -43,9 +43,6 @@
     <t>s2</t>
   </si>
   <si>
-    <t>s3</t>
-  </si>
-  <si>
     <t>s1</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>p2</t>
   </si>
   <si>
-    <t>p3</t>
-  </si>
-  <si>
     <t>TC3_twitLoginChrome</t>
   </si>
   <si>
@@ -68,6 +62,9 @@
   </si>
   <si>
     <t>https://twitter.com/login?lang=en</t>
+  </si>
+  <si>
+    <t>Tcs@1983</t>
   </si>
 </sst>
 </file>
@@ -439,7 +436,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +445,7 @@
     <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -464,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -475,7 +472,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -484,18 +481,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -504,18 +501,18 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -524,18 +521,18 @@
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9967887510</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -544,17 +541,21 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9967887510</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to reflection code 01 Dec 2019
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,12 +550,33 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9967887510</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1"/>
     <hyperlink ref="F5" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>